<commit_message>
Can perform on any number of models
</commit_message>
<xml_diff>
--- a/Data Model.xlsx
+++ b/Data Model.xlsx
@@ -5,6 +5,9 @@
   <sheets>
     <sheet state="visible" name="user" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="product" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Sheet4" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Sheet5" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="50">
   <si>
     <t>key</t>
   </si>
@@ -140,9 +143,6 @@
     <t>Total Number of orders completed for this product</t>
   </si>
   <si>
-    <t>status -</t>
-  </si>
-  <si>
     <t>1 Active
 0 disabled
 -1 Deleted</t>
@@ -180,10 +180,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -203,12 +209,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000FF"/>
+        <bgColor rgb="FF0000FF"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -237,23 +249,40 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -268,6 +297,18 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -479,7 +520,7 @@
     <col customWidth="1" min="7" max="7" width="20.75"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="25.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,117 +542,145 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="C2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="C3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="C4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="C5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
         <v>1.0</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="F5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
     </row>
     <row r="7">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
     </row>
     <row r="8">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
     </row>
     <row r="9">
-      <c r="A9" s="1"/>
+      <c r="A9" s="7"/>
     </row>
     <row r="10">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
     </row>
     <row r="11">
-      <c r="A11" s="1"/>
+      <c r="A11" s="7"/>
     </row>
     <row r="12">
-      <c r="A12" s="1"/>
+      <c r="A12" s="7"/>
     </row>
     <row r="13">
-      <c r="A13" s="1"/>
+      <c r="A13" s="7"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -629,351 +698,466 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="13.88"/>
+    <col customWidth="1" min="7" max="7" width="22.75"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="C2" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="C3" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="C4" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="C5" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="C6" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="C7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="5" t="s">
+      <c r="C8" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="C9" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="3">
+      <c r="C10" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6">
         <v>0.0</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="E10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1.0</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="F11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="3" t="s">
+      <c r="C12" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="3" t="s">
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="3" t="s">
+      <c r="C14" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="3" t="s">
+    </row>
+    <row r="15">
+      <c r="A15" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="3" t="s">
+      <c r="C15" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>50</v>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>